<commit_message>
use privat lists for var names
</commit_message>
<xml_diff>
--- a/dic_itrf.xlsx
+++ b/dic_itrf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurgenwilbert/Dropbox/08-R/scaledic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705B4963-D9B6-A247-8C06-B28F2A9FDED2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF629C5A-D901-394A-BCE7-D4C784EA71FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="118">
   <si>
     <t>label</t>
   </si>
@@ -79,9 +79,6 @@
     <t>0:3</t>
   </si>
   <si>
-    <t>0 = Verhalten ist nicht problematisch; 1 = Verhalten ist leicht problematisch; 2 = Verhalten ist mäßig problematisch; 3 = Verhalten ist stark problematisch</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -361,9 +358,6 @@
     <t>MA</t>
   </si>
   <si>
-    <t>MA_NE</t>
-  </si>
-  <si>
     <t>SH</t>
   </si>
   <si>
@@ -371,6 +365,15 @@
   </si>
   <si>
     <t>ITRF</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>0 = not problematic; 1 = slightly problematic; 2 = problematic; 3 = strongly problematic</t>
+  </si>
+  <si>
+    <t>Casale et al. (2017)</t>
   </si>
 </sst>
 </file>
@@ -704,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C41"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -715,11 +718,11 @@
     <col min="6" max="6" width="46.83203125" customWidth="1"/>
     <col min="7" max="7" width="29.1640625" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" customWidth="1"/>
     <col min="12" max="12" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -757,24 +760,27 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -783,13 +789,13 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -801,39 +807,45 @@
         <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M2">
+        <v>-99</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -842,39 +854,45 @@
         <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M3">
+        <v>-99</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -883,21 +901,27 @@
         <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M4">
+        <v>-99</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -906,16 +930,16 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -924,21 +948,27 @@
         <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M5">
+        <v>-99</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -947,16 +977,16 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -965,21 +995,27 @@
         <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M6">
+        <v>-99</v>
+      </c>
+      <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -988,16 +1024,16 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1006,40 +1042,46 @@
         <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M7">
+        <v>-99</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" t="s">
-        <v>27</v>
-      </c>
       <c r="J8">
         <v>1</v>
       </c>
@@ -1047,39 +1089,45 @@
         <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M8">
+        <v>-99</v>
+      </c>
+      <c r="N8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1088,39 +1136,45 @@
         <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M9">
+        <v>-99</v>
+      </c>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1129,39 +1183,45 @@
         <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M10">
+        <v>-99</v>
+      </c>
+      <c r="N10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1170,39 +1230,45 @@
         <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M11">
+        <v>-99</v>
+      </c>
+      <c r="N11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1211,39 +1277,45 @@
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M12">
+        <v>-99</v>
+      </c>
+      <c r="N12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1252,39 +1324,45 @@
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M13">
+        <v>-99</v>
+      </c>
+      <c r="N13" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1293,39 +1371,45 @@
         <v>18</v>
       </c>
       <c r="L14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M14">
+        <v>-99</v>
+      </c>
+      <c r="N14" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1334,39 +1418,45 @@
         <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M15">
+        <v>-99</v>
+      </c>
+      <c r="N15" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1375,21 +1465,27 @@
         <v>18</v>
       </c>
       <c r="L16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M16">
+        <v>-99</v>
+      </c>
+      <c r="N16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1398,16 +1494,16 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1416,39 +1512,45 @@
         <v>18</v>
       </c>
       <c r="L17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M17">
+        <v>-99</v>
+      </c>
+      <c r="N17" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1457,39 +1559,45 @@
         <v>18</v>
       </c>
       <c r="L18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M18">
+        <v>-99</v>
+      </c>
+      <c r="N18" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1498,39 +1606,45 @@
         <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M19">
+        <v>-99</v>
+      </c>
+      <c r="N19" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1539,40 +1653,46 @@
         <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M20">
+        <v>-99</v>
+      </c>
+      <c r="N20" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" t="s">
         <v>40</v>
       </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" t="s">
-        <v>111</v>
-      </c>
-      <c r="I21" t="s">
-        <v>41</v>
-      </c>
       <c r="J21">
         <v>1</v>
       </c>
@@ -1580,36 +1700,39 @@
         <v>18</v>
       </c>
       <c r="L21" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M21">
+        <v>-99</v>
+      </c>
+      <c r="N21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="E22" t="s">
-        <v>113</v>
-      </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -1618,39 +1741,45 @@
         <v>18</v>
       </c>
       <c r="L22" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M22">
+        <v>-99</v>
+      </c>
+      <c r="N22" t="s">
+        <v>19</v>
+      </c>
+      <c r="O22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -1659,39 +1788,45 @@
         <v>18</v>
       </c>
       <c r="L23" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M23">
+        <v>-99</v>
+      </c>
+      <c r="N23" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -1700,115 +1835,133 @@
         <v>18</v>
       </c>
       <c r="L24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M24">
+        <v>-99</v>
+      </c>
+      <c r="N24" t="s">
+        <v>19</v>
+      </c>
+      <c r="O24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" t="s">
+        <v>116</v>
+      </c>
+      <c r="M25">
+        <v>-99</v>
+      </c>
+      <c r="N25" t="s">
+        <v>19</v>
+      </c>
+      <c r="O25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" t="s">
         <v>103</v>
       </c>
-      <c r="I25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="H26" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26">
+        <v>-99</v>
+      </c>
+      <c r="N26" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>87</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26" t="s">
-        <v>47</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="K26" t="s">
-        <v>18</v>
-      </c>
-      <c r="L26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>88</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -1817,39 +1970,45 @@
         <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M27">
+        <v>-99</v>
+      </c>
+      <c r="N27" t="s">
+        <v>19</v>
+      </c>
+      <c r="O27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -1858,39 +2017,45 @@
         <v>18</v>
       </c>
       <c r="L28" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M28">
+        <v>-99</v>
+      </c>
+      <c r="N28" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -1899,39 +2064,45 @@
         <v>18</v>
       </c>
       <c r="L29" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M29">
+        <v>-99</v>
+      </c>
+      <c r="N29" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -1940,39 +2111,45 @@
         <v>18</v>
       </c>
       <c r="L30" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M30">
+        <v>-99</v>
+      </c>
+      <c r="N30" t="s">
+        <v>19</v>
+      </c>
+      <c r="O30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31">
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -1981,39 +2158,45 @@
         <v>18</v>
       </c>
       <c r="L31" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M31">
+        <v>-99</v>
+      </c>
+      <c r="N31" t="s">
+        <v>19</v>
+      </c>
+      <c r="O31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32">
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2022,39 +2205,45 @@
         <v>18</v>
       </c>
       <c r="L32" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M32">
+        <v>-99</v>
+      </c>
+      <c r="N32" t="s">
+        <v>19</v>
+      </c>
+      <c r="O32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2063,39 +2252,45 @@
         <v>18</v>
       </c>
       <c r="L33" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M33">
+        <v>-99</v>
+      </c>
+      <c r="N33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34">
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2104,39 +2299,45 @@
         <v>18</v>
       </c>
       <c r="L34" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M34">
+        <v>-99</v>
+      </c>
+      <c r="N34" t="s">
+        <v>19</v>
+      </c>
+      <c r="O34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2145,39 +2346,45 @@
         <v>18</v>
       </c>
       <c r="L35" t="s">
-        <v>19</v>
-      </c>
-      <c r="M35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M35">
+        <v>-99</v>
+      </c>
+      <c r="N35" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2186,39 +2393,45 @@
         <v>18</v>
       </c>
       <c r="L36" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M36">
+        <v>-99</v>
+      </c>
+      <c r="N36" t="s">
+        <v>19</v>
+      </c>
+      <c r="O36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37">
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -2227,39 +2440,45 @@
         <v>18</v>
       </c>
       <c r="L37" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M37">
+        <v>-99</v>
+      </c>
+      <c r="N37" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38">
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2268,39 +2487,45 @@
         <v>18</v>
       </c>
       <c r="L38" t="s">
-        <v>19</v>
-      </c>
-      <c r="M38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M38">
+        <v>-99</v>
+      </c>
+      <c r="N38" t="s">
+        <v>19</v>
+      </c>
+      <c r="O38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2309,83 +2534,95 @@
         <v>18</v>
       </c>
       <c r="L39" t="s">
-        <v>19</v>
-      </c>
-      <c r="M39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M39">
+        <v>-99</v>
+      </c>
+      <c r="N39" t="s">
+        <v>19</v>
+      </c>
+      <c r="O39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40">
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G40" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" t="s">
+        <v>116</v>
+      </c>
+      <c r="M40">
+        <v>-99</v>
+      </c>
+      <c r="N40" t="s">
+        <v>19</v>
+      </c>
+      <c r="O40" t="s">
+        <v>117</v>
+      </c>
+      <c r="P40" t="s">
         <v>104</v>
       </c>
-      <c r="H40" t="s">
-        <v>110</v>
-      </c>
-      <c r="I40" t="s">
-        <v>38</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>18</v>
-      </c>
-      <c r="L40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M40" t="s">
-        <v>20</v>
-      </c>
-      <c r="O40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41">
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -2394,10 +2631,16 @@
         <v>18</v>
       </c>
       <c r="L41" t="s">
-        <v>19</v>
-      </c>
-      <c r="M41" t="s">
-        <v>20</v>
+        <v>116</v>
+      </c>
+      <c r="M41">
+        <v>-99</v>
+      </c>
+      <c r="N41" t="s">
+        <v>19</v>
+      </c>
+      <c r="O41" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
item_label to item_name and item_label_short to item_label
</commit_message>
<xml_diff>
--- a/dic_itrf.xlsx
+++ b/dic_itrf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurgenwilbert/Dropbox/08-R/scaledic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24401C0F-50DD-6443-97E2-421F1623B285}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F295F9-8DAA-B24C-B935-2162AFC33689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -683,18 +683,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
     <col min="9" max="9" width="43.1640625" customWidth="1"/>
-    <col min="12" max="12" width="32.5" customWidth="1"/>
+    <col min="12" max="12" width="67.5" customWidth="1"/>
+    <col min="15" max="15" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -1640,7 +1642,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
internal renaming of variable names
</commit_message>
<xml_diff>
--- a/dic_itrf.xlsx
+++ b/dic_itrf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurgenwilbert/Dropbox/08-R/scaledic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F295F9-8DAA-B24C-B935-2162AFC33689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7B9AB4-3D07-3F4D-BD92-A9332855045F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="107">
   <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
     <t>Externalizing</t>
   </si>
   <si>
-    <t>Item double</t>
-  </si>
-  <si>
     <t>ITRF</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
     <t>0 = not problematic; 1 = slightly problematic; 2 = problematic; 3 = strongly problematic</t>
   </si>
   <si>
-    <t>SUB_SCALE_2</t>
-  </si>
-  <si>
     <t>Academic Productivity/Disorganization</t>
   </si>
   <si>
@@ -341,6 +332,15 @@
   </si>
   <si>
     <t>Volpe et al. et al. (unpublished)</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sub_scale_2</t>
+  </si>
+  <si>
+    <t>Item doubled</t>
   </si>
 </sst>
 </file>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="L26" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -693,7 +693,7 @@
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="30.5" customWidth="1"/>
+    <col min="8" max="8" width="32.5" customWidth="1"/>
     <col min="9" max="9" width="43.1640625" customWidth="1"/>
     <col min="12" max="12" width="67.5" customWidth="1"/>
     <col min="15" max="15" width="24.83203125" customWidth="1"/>
@@ -701,1747 +701,1747 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M2">
         <v>-99</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M3">
         <v>-99</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M4">
         <v>-99</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M5">
         <v>-99</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M6">
         <v>-99</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M7">
         <v>-99</v>
       </c>
       <c r="N7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M8">
         <v>-99</v>
       </c>
       <c r="N8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M9">
         <v>-99</v>
       </c>
       <c r="N9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M10">
         <v>-99</v>
       </c>
       <c r="N10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M11">
         <v>-99</v>
       </c>
       <c r="N11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M12">
         <v>-99</v>
       </c>
       <c r="N12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M13">
         <v>-99</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M14">
         <v>-99</v>
       </c>
       <c r="N14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M15">
         <v>-99</v>
       </c>
       <c r="N15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M16">
         <v>-99</v>
       </c>
       <c r="N16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M17">
         <v>-99</v>
       </c>
       <c r="N17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M18">
         <v>-99</v>
       </c>
       <c r="N18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M19">
         <v>-99</v>
       </c>
       <c r="N19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20">
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M20">
         <v>-99</v>
       </c>
       <c r="N20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" t="s">
         <v>38</v>
       </c>
-      <c r="E21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" t="s">
-        <v>98</v>
-      </c>
-      <c r="I21" t="s">
-        <v>39</v>
-      </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M21">
         <v>-99</v>
       </c>
       <c r="N21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M22">
         <v>-99</v>
       </c>
       <c r="N22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M23">
         <v>-99</v>
       </c>
       <c r="N23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M24">
         <v>-99</v>
       </c>
       <c r="N24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M25">
         <v>-99</v>
       </c>
       <c r="N25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J26">
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M26">
         <v>-99</v>
       </c>
       <c r="N26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M27">
         <v>-99</v>
       </c>
       <c r="N27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M28">
         <v>-99</v>
       </c>
       <c r="N28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29">
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M29">
         <v>-99</v>
       </c>
       <c r="N29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M30">
         <v>-99</v>
       </c>
       <c r="N30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31">
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M31">
         <v>-99</v>
       </c>
       <c r="N31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32">
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J32">
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M32">
         <v>-99</v>
       </c>
       <c r="N32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33">
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M33">
         <v>-99</v>
       </c>
       <c r="N33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34">
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J34">
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M34">
         <v>-99</v>
       </c>
       <c r="N34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J35">
         <v>1</v>
       </c>
       <c r="K35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M35">
         <v>-99</v>
       </c>
       <c r="N35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O35" t="s">
+        <v>103</v>
+      </c>
+      <c r="P35" t="s">
         <v>106</v>
-      </c>
-      <c r="P35" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36">
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J36">
         <v>1</v>
       </c>
       <c r="K36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M36">
         <v>-99</v>
       </c>
       <c r="N36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37">
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J37">
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M37">
         <v>-99</v>
       </c>
       <c r="N37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
impute missing in apply_dic
</commit_message>
<xml_diff>
--- a/dic_itrf.xlsx
+++ b/dic_itrf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurgenwilbert/Dropbox/08-R/scaledic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBE05B6-163C-FB46-B4C2-DF6CCE6D760A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35E9C09-FBBE-6C46-976A-6936E775FE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="120">
   <si>
     <t>index</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>item</t>
-  </si>
-  <si>
-    <t>factor</t>
   </si>
 </sst>
 </file>
@@ -719,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L18" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1797,7 +1794,7 @@
         <v>-99</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>99</v>

</xml_diff>